<commit_message>
In standby : Priority feature on rooms service
</commit_message>
<xml_diff>
--- a/tests/nrt1/input_nrt1.xlsx
+++ b/tests/nrt1/input_nrt1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS5997\src\neonat\tests\nrt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCC5C1E-8899-47D4-AF97-44C6C05EEC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E823196-C842-4A0A-A1ED-020E898409DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
   <si>
     <t>services</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>r13</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
@@ -625,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE173FA1-E983-499D-AB64-6CD8215CA3C5}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:G14"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,7 +645,7 @@
     <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -664,8 +667,11 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -685,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -705,7 +711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -725,7 +731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -745,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -765,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -785,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -805,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -819,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -833,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -847,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -864,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -881,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -898,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Correction : if there is more places than babies, ensure that a baby has only one room
</commit_message>
<xml_diff>
--- a/tests/nrt1/input_nrt1.xlsx
+++ b/tests/nrt1/input_nrt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS5997\src\neonat\tests\nrt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FE13FC-1285-4911-B911-C62C9D72F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCC5C1E-8899-47D4-AF97-44C6C05EEC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1464" windowWidth="17280" windowHeight="7764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="babies" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
   <si>
     <t>services</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>rea,soins,neo</t>
+  </si>
+  <si>
+    <t>r11</t>
+  </si>
+  <si>
+    <t>r12</t>
+  </si>
+  <si>
+    <t>r13</t>
   </si>
 </sst>
 </file>
@@ -473,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFF5F45-CFAD-4E61-9970-5F5BE534E7C0}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+    <sheetView zoomScale="102" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -616,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE173FA1-E983-499D-AB64-6CD8215CA3C5}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,17 +847,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a treatment feature : babies should have a room with the specific treatment they need
</commit_message>
<xml_diff>
--- a/tests/nrt1/input_nrt1.xlsx
+++ b/tests/nrt1/input_nrt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS5997\src\neonat\tests\nrt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E823196-C842-4A0A-A1ED-020E898409DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220FAA90-ECC3-4D4E-8586-0E18D6DCCBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="babies" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
   <si>
     <t>services</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>priority</t>
+  </si>
+  <si>
+    <t>treatment</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFF5F45-CFAD-4E61-9970-5F5BE534E7C0}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,7 +502,7 @@
     <col min="6" max="6" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -509,8 +512,11 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -521,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -532,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -543,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -554,7 +560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -565,7 +571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -576,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -587,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -598,7 +604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -609,7 +615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -628,10 +634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE173FA1-E983-499D-AB64-6CD8215CA3C5}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="103" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +651,7 @@
     <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -670,8 +676,11 @@
       <c r="H1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -691,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -711,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -731,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -751,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -771,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -791,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -811,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -825,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -839,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -853,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -870,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -887,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -904,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
[DC] Include controllers to ensure that the Excel file has no errors in its data : missing element of set, or spelling mistake
</commit_message>
<xml_diff>
--- a/tests/nrt1/input_nrt1.xlsx
+++ b/tests/nrt1/input_nrt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VS5997\src\neonat\tests\nrt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220FAA90-ECC3-4D4E-8586-0E18D6DCCBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3CE6FA-582F-4BF3-B3AF-57D8F411FBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="babies" sheetId="2" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>